<commit_message>
rtl and c code
</commit_message>
<xml_diff>
--- a/proj_asic/docs/register_map.xlsx
+++ b/proj_asic/docs/register_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8055" windowHeight="5550"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20595" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="127">
   <si>
     <t>Register Name</t>
   </si>
@@ -174,33 +174,15 @@
     <t>0x010</t>
   </si>
   <si>
-    <t>0x040</t>
-  </si>
-  <si>
-    <t>0x43C</t>
-  </si>
-  <si>
-    <t>0x044</t>
-  </si>
-  <si>
     <t>address register used for indirect addressing via i2c</t>
   </si>
   <si>
     <t>0x014</t>
   </si>
   <si>
-    <t>I2C_REG_INDIR_DATA</t>
-  </si>
-  <si>
     <t>I2C_REG_INDIR_ADDR</t>
   </si>
   <si>
-    <t>data access register</t>
-  </si>
-  <si>
-    <t>ro_i2c_reg_indir_data</t>
-  </si>
-  <si>
     <t>rf_filter_shift</t>
   </si>
   <si>
@@ -225,9 +207,6 @@
     <t>half of the clock frequency divided by this #</t>
   </si>
   <si>
-    <t>0x018</t>
-  </si>
-  <si>
     <t>0x1</t>
   </si>
   <si>
@@ -282,18 +261,12 @@
     <t>11:0</t>
   </si>
   <si>
-    <t>8:0</t>
-  </si>
-  <si>
     <t>11:8</t>
   </si>
   <si>
     <t>15:12</t>
   </si>
   <si>
-    <t>19:12</t>
-  </si>
-  <si>
     <t>31:20</t>
   </si>
   <si>
@@ -378,40 +351,55 @@
     <t>rf_filter_coeef510_b</t>
   </si>
   <si>
+    <t>rf_filter_coeef511_a</t>
+  </si>
+  <si>
     <t>rf_filter_coeef511_b</t>
   </si>
   <si>
-    <t>0x041</t>
-  </si>
-  <si>
-    <t>0x042</t>
-  </si>
-  <si>
-    <t>0x043</t>
-  </si>
-  <si>
-    <t>0x045</t>
-  </si>
-  <si>
-    <t>0x046</t>
-  </si>
-  <si>
-    <t>0x047</t>
-  </si>
-  <si>
-    <t>0x043C</t>
-  </si>
-  <si>
-    <t>0x043D</t>
-  </si>
-  <si>
-    <t>0x043E</t>
-  </si>
-  <si>
-    <t>0x043F</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>0x001</t>
+  </si>
+  <si>
+    <t>19:8</t>
+  </si>
+  <si>
+    <t>0x0400</t>
+  </si>
+  <si>
+    <t>0x0401</t>
+  </si>
+  <si>
+    <t>0x0402</t>
+  </si>
+  <si>
+    <t>0x0403</t>
+  </si>
+  <si>
+    <t>0x0404</t>
+  </si>
+  <si>
+    <t>0x0405</t>
+  </si>
+  <si>
+    <t>0x0406</t>
+  </si>
+  <si>
+    <t>0x0407</t>
+  </si>
+  <si>
+    <t>0x7FC</t>
+  </si>
+  <si>
+    <t>0x07FD</t>
+  </si>
+  <si>
+    <t>0x07FC</t>
+  </si>
+  <si>
+    <t>0x07FE</t>
+  </si>
+  <si>
+    <t>0x07FF</t>
   </si>
 </sst>
 </file>
@@ -834,7 +822,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -842,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +886,9 @@
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -920,7 +910,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
         <v>29</v>
@@ -961,13 +953,13 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>18</v>
@@ -985,13 +977,13 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>20</v>
@@ -1000,7 +992,7 @@
         <v>19</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1009,22 +1001,22 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1033,42 +1025,42 @@
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>19</v>
@@ -1077,27 +1069,27 @@
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>19</v>
@@ -1111,7 +1103,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
@@ -1129,31 +1121,31 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="2"/>
@@ -1161,10 +1153,10 @@
         <v>19</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1187,13 +1179,13 @@
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>44</v>
@@ -1211,13 +1203,13 @@
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>28</v>
@@ -1235,16 +1227,16 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>45</v>
@@ -1259,16 +1251,16 @@
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>10</v>
@@ -1300,74 +1292,74 @@
         <v>29</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="13" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="13" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>50</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="13" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>24</v>
@@ -1381,32 +1373,26 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>103</v>
-      </c>
       <c r="E25" s="13"/>
-      <c r="F25" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>49</v>
-      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="9"/>
@@ -1417,20 +1403,20 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>19</v>
@@ -1441,18 +1427,18 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>19</v>
@@ -1462,71 +1448,81 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="A29" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>46</v>
+      <c r="A30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="A31" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>19</v>
@@ -1537,18 +1533,18 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>19</v>
@@ -1558,81 +1554,81 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="7" t="s">
+      <c r="A34" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="7" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>19</v>
@@ -1643,18 +1639,18 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>19</v>
@@ -1664,81 +1660,81 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" s="2" t="s">
+      <c r="B40" s="7"/>
+      <c r="C40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="2" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>19</v>
@@ -1749,18 +1745,18 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>19</v>
@@ -1770,56 +1766,10 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E47" s="1"/>
+      <c r="E45" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed chip.v Interface Issues
</commit_message>
<xml_diff>
--- a/proj_asic/docs/register_map.xlsx
+++ b/proj_asic/docs/register_map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="106">
   <si>
     <t>Register Name</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>4:2</t>
+  </si>
+  <si>
+    <t>6:6</t>
+  </si>
+  <si>
+    <t>rf_i2si_en</t>
   </si>
 </sst>
 </file>
@@ -766,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,38 +965,32 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -998,19 +998,19 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1019,19 +1019,19 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>41</v>
+        <v>10</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1040,19 +1040,19 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1061,19 +1061,19 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="4" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>41</v>
+        <v>10</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1082,182 +1082,182 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G17" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>64</v>
-      </c>
+      <c r="A23" s="15"/>
       <c r="B23" s="11"/>
       <c r="C23" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>30</v>
@@ -1271,17 +1271,17 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>19</v>
@@ -1292,14 +1292,14 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>31</v>
@@ -1312,49 +1312,49 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>33</v>
@@ -1368,17 +1368,17 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>19</v>
@@ -1389,14 +1389,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>34</v>
@@ -1409,49 +1409,49 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>36</v>
@@ -1465,17 +1465,17 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>19</v>
@@ -1486,14 +1486,14 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>37</v>
@@ -1502,6 +1502,27 @@
         <v>19</v>
       </c>
       <c r="G38" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>